<commit_message>
multiple plot problem fixed
</commit_message>
<xml_diff>
--- a/Import/pyControllerList/Storage Controller.xlsx
+++ b/Import/pyControllerList/Storage Controller.xlsx
@@ -1282,14 +1282,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
     <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
@@ -1458,7 +1458,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>23</v>

</xml_diff>